<commit_message>
Test ecryptPassword y update Memoria
</commit_message>
<xml_diff>
--- a/Docs/planificacion.xlsx
+++ b/Docs/planificacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frangabarda\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frangabarda\Documents\GitHub\ProyectoFinalDAM\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{933C67B7-F13C-458A-BC37-6388C912DEA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DD9486-3642-41D9-BCE2-4BE6EA443BBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{76274755-38AF-4643-BA66-2F828881DD86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
   <si>
     <t>Semana</t>
   </si>
@@ -190,13 +190,31 @@
   </si>
   <si>
     <t>Redacción de la memoria (conclusiones y resumen)</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>LINEA DE TIEMPO</t>
+  </si>
+  <si>
+    <t>Diseño de la arquitectura del sistema</t>
+  </si>
+  <si>
+    <t>Redacción de la memoria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,16 +222,88 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3B67B7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4874C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5D84CB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF365FA8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF305494"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -221,18 +311,118 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF5D84CB"/>
+      <color rgb="FF8EA9DB"/>
+      <color rgb="FF305494"/>
+      <color rgb="FF365FA8"/>
+      <color rgb="FF3B67B7"/>
+      <color rgb="FF4874C4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -541,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FC20BA-846D-4CCE-AC8A-8FDAD5F13FCE}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:AF42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH10" sqref="AH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,409 +742,1003 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="46.140625" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="59.5703125" customWidth="1"/>
+    <col min="7" max="18" width="4.85546875" customWidth="1"/>
+    <col min="20" max="20" width="61.42578125" customWidth="1"/>
+    <col min="21" max="32" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="T1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="12"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>3</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>3</v>
+      </c>
+      <c r="R3" s="2">
+        <v>4</v>
+      </c>
+      <c r="T3" s="8"/>
+      <c r="U3" s="7">
+        <v>1</v>
+      </c>
+      <c r="V3" s="7">
+        <v>2</v>
+      </c>
+      <c r="W3" s="7">
+        <v>3</v>
+      </c>
+      <c r="X3" s="7">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="7">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="7">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="7">
+        <v>3</v>
+      </c>
+      <c r="AF3" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="T4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="13"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+    </row>
+    <row r="5" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="T5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+    </row>
+    <row r="6" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="T6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+    </row>
+    <row r="7" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
       <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="T7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+    </row>
+    <row r="8" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+    </row>
+    <row r="9" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>11</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>14</v>
       </c>
       <c r="D9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+    </row>
+    <row r="10" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+    </row>
+    <row r="11" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+    </row>
+    <row r="12" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+    </row>
+    <row r="13" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="16"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+    </row>
+    <row r="14" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
+      <c r="D14">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+    </row>
+    <row r="15" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="5"/>
+    </row>
+    <row r="16" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>19</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>21</v>
       </c>
       <c r="D16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+    </row>
+    <row r="17" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+    </row>
+    <row r="18" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="5"/>
+    </row>
+    <row r="19" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+      <c r="T19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="5"/>
+    </row>
+    <row r="20" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>6</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="T20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="16"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="19"/>
+    </row>
+    <row r="21" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>24</v>
-      </c>
-      <c r="D19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
       </c>
       <c r="D21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="20"/>
+    </row>
+    <row r="22" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="16"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="20"/>
+    </row>
+    <row r="23" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>8</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>29</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>30</v>
-      </c>
-      <c r="D25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
       </c>
       <c r="D27">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>33</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>49</v>
       </c>
-      <c r="D29">
+      <c r="D31">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>10</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C32" t="s">
         <v>35</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>36</v>
-      </c>
-      <c r="D31">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>11</v>
-      </c>
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
       </c>
       <c r="D33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>20</v>
+      </c>
+      <c r="F35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>39</v>
       </c>
-      <c r="D34">
+      <c r="D36">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>40</v>
-      </c>
-      <c r="D35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>12</v>
-      </c>
-      <c r="B37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" t="s">
-        <v>52</v>
       </c>
       <c r="D37">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
         <v>42</v>
       </c>
-      <c r="D38">
+      <c r="D40">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+      <c r="F40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>53</v>
       </c>
-      <c r="D39">
+      <c r="D41">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+      <c r="F41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>54</v>
       </c>
-      <c r="D40">
+      <c r="D42">
         <v>10</v>
       </c>
+      <c r="F42" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D40">
-    <cfRule type="colorScale" priority="1">
+  <mergeCells count="9">
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="G1:R1"/>
+    <mergeCell ref="U1:AF1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="T1:T3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:D42">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F42">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:T42 T1">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>